<commit_message>
ssh key instructions added
</commit_message>
<xml_diff>
--- a/Git_commands.xlsx
+++ b/Git_commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\repo\self-study\pluralsight\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\self-study-git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B055E1-C63A-461A-91C7-222F7184CACC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DD9D69-BA35-44FB-90E5-7D6A208ECE64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" tabRatio="816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="108">
   <si>
     <t>git touch mynewfile.txt</t>
   </si>
@@ -359,12 +359,39 @@
   <si>
     <t>https://code.visualstudio.com/docs/getstarted/tips-and-tricks</t>
   </si>
+  <si>
+    <t>Connecting to GitHub with SSH</t>
+  </si>
+  <si>
+    <t>ssh-keygen -o -a 100 -t ed25519 -f ~/.ssh/id_ed25519 -C "mkrstv@gmail.com"</t>
+  </si>
+  <si>
+    <t>generates the key</t>
+  </si>
+  <si>
+    <t>eval `ssh-agent -s`</t>
+  </si>
+  <si>
+    <t>start the ssh-agent in the background</t>
+  </si>
+  <si>
+    <t>passphrase</t>
+  </si>
+  <si>
+    <t>LeeMu</t>
+  </si>
+  <si>
+    <t>clip &lt; ~/.ssh/id_ed25519.pub</t>
+  </si>
+  <si>
+    <t>Copy the SSH public key to your clipboard</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +459,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -502,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,10 +563,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,28 +848,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="79.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="48" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.109375" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="17.25">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>97</v>
       </c>
     </row>
@@ -949,90 +984,122 @@
       </c>
       <c r="C16" s="14"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>93</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="14"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="14"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>96</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="14"/>
     </row>
-    <row r="23" spans="1:3" ht="15">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="15">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="31" spans="1:3" ht="20.399999999999999">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.399999999999999">
+    <row r="27" spans="1:4">
+      <c r="A27" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:2" ht="20.399999999999999">
+    <row r="33" spans="1:2" ht="21">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:2" ht="20.399999999999999">
+    <row r="34" spans="1:2" ht="21">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:2" ht="20.399999999999999">
+    <row r="35" spans="1:2" ht="21">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:2" ht="20.399999999999999">
+    <row r="36" spans="1:2" ht="21">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:2" ht="20.399999999999999">
+    <row r="37" spans="1:2" ht="21">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:2" ht="20.399999999999999">
+    <row r="38" spans="1:2" ht="21">
       <c r="A38" s="2"/>
     </row>
-    <row r="41" spans="1:2" ht="20.399999999999999">
+    <row r="41" spans="1:2" ht="21">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="20.399999999999999">
+    <row r="44" spans="1:2" ht="21">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -1045,7 +1112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.6" thickBot="1">
+    <row r="46" spans="1:2" ht="15.75" thickBot="1">
       <c r="A46" s="4" t="s">
         <v>15</v>
       </c>
@@ -1053,7 +1120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.6" thickBot="1">
+    <row r="47" spans="1:2" ht="15.75" thickBot="1">
       <c r="A47" s="5" t="s">
         <v>17</v>
       </c>
@@ -1061,7 +1128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.6" thickBot="1">
+    <row r="48" spans="1:2" ht="15.75" thickBot="1">
       <c r="A48" s="7" t="s">
         <v>19</v>
       </c>
@@ -1088,13 +1155,13 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2">
+    <row r="1" spans="1:2" ht="17.25">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1110,11 +1177,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" ht="15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1122,11 +1189,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" ht="15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,115 +1201,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" ht="15">
+    <row r="17" spans="1:2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" ht="15">
+    <row r="18" spans="1:2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" ht="15">
+    <row r="19" spans="1:2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" ht="15">
+    <row r="20" spans="1:2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="15">
+    <row r="21" spans="1:2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="15">
+    <row r="22" spans="1:2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="15">
+    <row r="23" spans="1:2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" ht="15">
+    <row r="24" spans="1:2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="15">
+    <row r="25" spans="1:2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="15">
+    <row r="26" spans="1:2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="15">
+    <row r="27" spans="1:2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="15">
+    <row r="28" spans="1:2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="15">
+    <row r="29" spans="1:2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="15">
+    <row r="30" spans="1:2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="15">
+    <row r="31" spans="1:2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="15">
+    <row r="32" spans="1:2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" ht="15">
+    <row r="33" spans="1:2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15">
+    <row r="34" spans="1:2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
@@ -1261,13 +1328,13 @@
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2">
+    <row r="1" spans="1:2" ht="17.25">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -1320,25 +1387,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="20.399999999999999">
+    <row r="20" spans="1:1" ht="21">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" ht="20.399999999999999">
+    <row r="21" spans="1:1" ht="21">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" ht="20.399999999999999">
+    <row r="22" spans="1:1" ht="21">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" ht="20.399999999999999">
+    <row r="23" spans="1:1" ht="21">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" ht="20.399999999999999">
+    <row r="24" spans="1:1" ht="21">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" ht="20.399999999999999">
+    <row r="25" spans="1:1" ht="21">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1" ht="20.399999999999999">
+    <row r="26" spans="1:1" ht="21">
       <c r="A26" s="2"/>
     </row>
   </sheetData>
@@ -1356,13 +1423,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2">
+    <row r="1" spans="1:2" ht="17.25">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -1504,13 +1571,13 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="85.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2">
+    <row r="1" spans="1:2" ht="17.25">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -1580,13 +1647,13 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2">
+    <row r="1" spans="1:2" ht="17.25">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>

</xml_diff>